<commit_message>
switch quarto format and fix references
</commit_message>
<xml_diff>
--- a/paper/supplements/S1-md_40_V24-DJH.xlsx
+++ b/paper/supplements/S1-md_40_V24-DJH.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danhicks/Google Drive/Coding/*race-science/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danhicks/Google Drive/Coding/*race-science/paper/supplements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE021F3-A4DC-5F49-8EF4-59D02AF2950D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A1FB74-3690-104F-B7A5-91A796597E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="16860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4754,18 +4754,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{14CDDFB3-4362-004D-849A-D3522D864070}" name="Table1" displayName="Table1" ref="A1:N344" totalsRowShown="0" headerRowDxfId="9">
-  <autoFilter ref="A1:N344" xr:uid="{14CDDFB3-4362-004D-849A-D3522D864070}">
-    <filterColumn colId="1">
-      <customFilters>
-        <customFilter operator="greaterThan" val="0.97"/>
-      </customFilters>
-    </filterColumn>
-    <filterColumn colId="9">
-      <filters>
-        <filter val="n"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:N344" xr:uid="{14CDDFB3-4362-004D-849A-D3522D864070}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{BE50ADC0-9941-1047-A040-0DD307282BE2}" name="topic" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{187918EF-F492-7E4E-9217-B43E987B1206}" name="gamma" dataDxfId="7"/>
@@ -5095,8 +5084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N344"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F75" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="K111" sqref="K111"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5160,7 +5149,7 @@
         <v>1512</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -5193,7 +5182,7 @@
       </c>
       <c r="N2"/>
     </row>
-    <row r="3" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -5226,7 +5215,7 @@
       </c>
       <c r="N3"/>
     </row>
-    <row r="4" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -5259,7 +5248,7 @@
       </c>
       <c r="N4"/>
     </row>
-    <row r="5" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -5292,7 +5281,7 @@
       </c>
       <c r="N5"/>
     </row>
-    <row r="6" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -5325,7 +5314,7 @@
       </c>
       <c r="N6"/>
     </row>
-    <row r="7" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -5358,7 +5347,7 @@
       </c>
       <c r="N7"/>
     </row>
-    <row r="8" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -5391,7 +5380,7 @@
       </c>
       <c r="N8"/>
     </row>
-    <row r="9" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -5424,7 +5413,7 @@
       </c>
       <c r="N9"/>
     </row>
-    <row r="10" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -5457,7 +5446,7 @@
       </c>
       <c r="N10"/>
     </row>
-    <row r="11" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -5490,7 +5479,7 @@
       </c>
       <c r="N11"/>
     </row>
-    <row r="12" spans="1:14" ht="64" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>9</v>
       </c>
@@ -5523,7 +5512,7 @@
       </c>
       <c r="N12"/>
     </row>
-    <row r="13" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>9</v>
       </c>
@@ -5556,7 +5545,7 @@
       </c>
       <c r="N13"/>
     </row>
-    <row r="14" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>9</v>
       </c>
@@ -5589,7 +5578,7 @@
       </c>
       <c r="N14"/>
     </row>
-    <row r="15" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>9</v>
       </c>
@@ -5622,7 +5611,7 @@
       </c>
       <c r="N15"/>
     </row>
-    <row r="16" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>9</v>
       </c>
@@ -5689,7 +5678,7 @@
         <v>1516</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>9</v>
       </c>
@@ -5722,7 +5711,7 @@
       </c>
       <c r="N18"/>
     </row>
-    <row r="19" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>9</v>
       </c>
@@ -5755,7 +5744,7 @@
       </c>
       <c r="N19"/>
     </row>
-    <row r="20" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>9</v>
       </c>
@@ -5788,7 +5777,7 @@
       </c>
       <c r="N20"/>
     </row>
-    <row r="21" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>9</v>
       </c>
@@ -5821,7 +5810,7 @@
       </c>
       <c r="N21"/>
     </row>
-    <row r="22" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>9</v>
       </c>
@@ -5854,7 +5843,7 @@
       </c>
       <c r="N22"/>
     </row>
-    <row r="23" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>9</v>
       </c>
@@ -5887,7 +5876,7 @@
       </c>
       <c r="N23"/>
     </row>
-    <row r="24" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>9</v>
       </c>
@@ -5920,7 +5909,7 @@
       </c>
       <c r="N24"/>
     </row>
-    <row r="25" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>9</v>
       </c>
@@ -5953,7 +5942,7 @@
       </c>
       <c r="N25"/>
     </row>
-    <row r="26" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>9</v>
       </c>
@@ -5986,7 +5975,7 @@
       </c>
       <c r="N26"/>
     </row>
-    <row r="27" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>9</v>
       </c>
@@ -6019,7 +6008,7 @@
       </c>
       <c r="N27"/>
     </row>
-    <row r="28" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>9</v>
       </c>
@@ -6052,7 +6041,7 @@
       </c>
       <c r="N28"/>
     </row>
-    <row r="29" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>9</v>
       </c>
@@ -6085,7 +6074,7 @@
       </c>
       <c r="N29"/>
     </row>
-    <row r="30" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>9</v>
       </c>
@@ -6118,7 +6107,7 @@
       </c>
       <c r="N30"/>
     </row>
-    <row r="31" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>9</v>
       </c>
@@ -6151,7 +6140,7 @@
       </c>
       <c r="N31"/>
     </row>
-    <row r="32" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>9</v>
       </c>
@@ -6184,7 +6173,7 @@
       </c>
       <c r="N32"/>
     </row>
-    <row r="33" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>9</v>
       </c>
@@ -6217,7 +6206,7 @@
       </c>
       <c r="N33"/>
     </row>
-    <row r="34" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>9</v>
       </c>
@@ -6250,7 +6239,7 @@
       </c>
       <c r="N34"/>
     </row>
-    <row r="35" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>9</v>
       </c>
@@ -6283,7 +6272,7 @@
       </c>
       <c r="N35"/>
     </row>
-    <row r="36" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>9</v>
       </c>
@@ -6316,7 +6305,7 @@
       </c>
       <c r="N36"/>
     </row>
-    <row r="37" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>9</v>
       </c>
@@ -6351,7 +6340,7 @@
         <v>1534</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>9</v>
       </c>
@@ -6384,7 +6373,7 @@
       </c>
       <c r="N38"/>
     </row>
-    <row r="39" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>9</v>
       </c>
@@ -6417,7 +6406,7 @@
       </c>
       <c r="N39"/>
     </row>
-    <row r="40" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>9</v>
       </c>
@@ -6450,7 +6439,7 @@
       </c>
       <c r="N40"/>
     </row>
-    <row r="41" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>9</v>
       </c>
@@ -6483,7 +6472,7 @@
       </c>
       <c r="N41"/>
     </row>
-    <row r="42" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>9</v>
       </c>
@@ -6516,7 +6505,7 @@
       </c>
       <c r="N42"/>
     </row>
-    <row r="43" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>9</v>
       </c>
@@ -6584,7 +6573,7 @@
         <v>1517</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>9</v>
       </c>
@@ -6617,7 +6606,7 @@
       </c>
       <c r="N45"/>
     </row>
-    <row r="46" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>9</v>
       </c>
@@ -6685,7 +6674,7 @@
         <v>1518</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>9</v>
       </c>
@@ -6718,7 +6707,7 @@
       </c>
       <c r="N48"/>
     </row>
-    <row r="49" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>9</v>
       </c>
@@ -6751,7 +6740,7 @@
       </c>
       <c r="N49"/>
     </row>
-    <row r="50" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>9</v>
       </c>
@@ -6784,7 +6773,7 @@
       </c>
       <c r="N50"/>
     </row>
-    <row r="51" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>9</v>
       </c>
@@ -6817,7 +6806,7 @@
       </c>
       <c r="N51"/>
     </row>
-    <row r="52" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>9</v>
       </c>
@@ -6849,7 +6838,7 @@
         <v>1519</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>9</v>
       </c>
@@ -6882,7 +6871,7 @@
       </c>
       <c r="N53"/>
     </row>
-    <row r="54" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>9</v>
       </c>
@@ -6915,7 +6904,7 @@
       </c>
       <c r="N54"/>
     </row>
-    <row r="55" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>9</v>
       </c>
@@ -6948,7 +6937,7 @@
       </c>
       <c r="N55"/>
     </row>
-    <row r="56" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>9</v>
       </c>
@@ -7016,7 +7005,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>9</v>
       </c>
@@ -7049,7 +7038,7 @@
       </c>
       <c r="N58"/>
     </row>
-    <row r="59" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>9</v>
       </c>
@@ -7082,7 +7071,7 @@
       </c>
       <c r="N59"/>
     </row>
-    <row r="60" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>9</v>
       </c>
@@ -7115,7 +7104,7 @@
       </c>
       <c r="N60"/>
     </row>
-    <row r="61" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>9</v>
       </c>
@@ -7148,7 +7137,7 @@
       </c>
       <c r="N61"/>
     </row>
-    <row r="62" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>9</v>
       </c>
@@ -7181,7 +7170,7 @@
       </c>
       <c r="N62"/>
     </row>
-    <row r="63" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>9</v>
       </c>
@@ -7249,7 +7238,7 @@
         <v>1521</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>9</v>
       </c>
@@ -7282,7 +7271,7 @@
       </c>
       <c r="N65"/>
     </row>
-    <row r="66" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>9</v>
       </c>
@@ -7315,7 +7304,7 @@
       </c>
       <c r="N66"/>
     </row>
-    <row r="67" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>9</v>
       </c>
@@ -7348,7 +7337,7 @@
       </c>
       <c r="N67"/>
     </row>
-    <row r="68" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>9</v>
       </c>
@@ -7381,7 +7370,7 @@
       </c>
       <c r="N68"/>
     </row>
-    <row r="69" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>9</v>
       </c>
@@ -7414,7 +7403,7 @@
       </c>
       <c r="N69"/>
     </row>
-    <row r="70" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>9</v>
       </c>
@@ -7447,7 +7436,7 @@
       </c>
       <c r="N70"/>
     </row>
-    <row r="71" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>9</v>
       </c>
@@ -7479,7 +7468,7 @@
         <v>1522</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>9</v>
       </c>
@@ -7512,7 +7501,7 @@
       </c>
       <c r="N72"/>
     </row>
-    <row r="73" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>9</v>
       </c>
@@ -7545,7 +7534,7 @@
       </c>
       <c r="N73"/>
     </row>
-    <row r="74" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>9</v>
       </c>
@@ -7615,7 +7604,7 @@
         <v>1524</v>
       </c>
     </row>
-    <row r="76" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>9</v>
       </c>
@@ -7648,7 +7637,7 @@
       </c>
       <c r="N76"/>
     </row>
-    <row r="77" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>9</v>
       </c>
@@ -7681,7 +7670,7 @@
       </c>
       <c r="N77"/>
     </row>
-    <row r="78" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>9</v>
       </c>
@@ -7714,7 +7703,7 @@
       </c>
       <c r="N78"/>
     </row>
-    <row r="79" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>9</v>
       </c>
@@ -7747,7 +7736,7 @@
       </c>
       <c r="N79"/>
     </row>
-    <row r="80" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>9</v>
       </c>
@@ -7782,7 +7771,7 @@
         <v>1525</v>
       </c>
     </row>
-    <row r="81" spans="1:14" ht="64" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>9</v>
       </c>
@@ -7815,7 +7804,7 @@
       </c>
       <c r="N81"/>
     </row>
-    <row r="82" spans="1:14" ht="64" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>9</v>
       </c>
@@ -7848,7 +7837,7 @@
       </c>
       <c r="N82"/>
     </row>
-    <row r="83" spans="1:14" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>9</v>
       </c>
@@ -7881,7 +7870,7 @@
       </c>
       <c r="N83"/>
     </row>
-    <row r="84" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>9</v>
       </c>
@@ -7916,7 +7905,7 @@
         <v>1526</v>
       </c>
     </row>
-    <row r="85" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>9</v>
       </c>
@@ -7949,7 +7938,7 @@
       </c>
       <c r="N85"/>
     </row>
-    <row r="86" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>9</v>
       </c>
@@ -8017,7 +8006,7 @@
         <v>1535</v>
       </c>
     </row>
-    <row r="88" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
         <v>9</v>
       </c>
@@ -8083,7 +8072,7 @@
       </c>
       <c r="N89"/>
     </row>
-    <row r="90" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>9</v>
       </c>
@@ -8116,7 +8105,7 @@
       </c>
       <c r="N90"/>
     </row>
-    <row r="91" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>9</v>
       </c>
@@ -8182,7 +8171,7 @@
       </c>
       <c r="N92"/>
     </row>
-    <row r="93" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>9</v>
       </c>
@@ -8215,7 +8204,7 @@
       </c>
       <c r="N93"/>
     </row>
-    <row r="94" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
         <v>9</v>
       </c>
@@ -8248,7 +8237,7 @@
       </c>
       <c r="N94"/>
     </row>
-    <row r="95" spans="1:14" ht="64" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
         <v>9</v>
       </c>
@@ -8281,7 +8270,7 @@
       </c>
       <c r="N95"/>
     </row>
-    <row r="96" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
         <v>9</v>
       </c>
@@ -8314,7 +8303,7 @@
       </c>
       <c r="N96"/>
     </row>
-    <row r="97" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>9</v>
       </c>
@@ -8349,7 +8338,7 @@
         <v>1527</v>
       </c>
     </row>
-    <row r="98" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>9</v>
       </c>
@@ -8382,7 +8371,7 @@
       </c>
       <c r="N98"/>
     </row>
-    <row r="99" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>9</v>
       </c>
@@ -8453,7 +8442,7 @@
         <v>1528</v>
       </c>
     </row>
-    <row r="101" spans="1:14" ht="64" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>9</v>
       </c>
@@ -8486,7 +8475,7 @@
       </c>
       <c r="N101"/>
     </row>
-    <row r="102" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>9</v>
       </c>
@@ -8519,7 +8508,7 @@
       </c>
       <c r="N102"/>
     </row>
-    <row r="103" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>9</v>
       </c>
@@ -8552,7 +8541,7 @@
       </c>
       <c r="N103"/>
     </row>
-    <row r="104" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>9</v>
       </c>
@@ -8585,7 +8574,7 @@
       </c>
       <c r="N104"/>
     </row>
-    <row r="105" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>9</v>
       </c>
@@ -8618,7 +8607,7 @@
       </c>
       <c r="N105"/>
     </row>
-    <row r="106" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>9</v>
       </c>
@@ -8651,7 +8640,7 @@
       </c>
       <c r="N106"/>
     </row>
-    <row r="107" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>9</v>
       </c>
@@ -8719,7 +8708,7 @@
         <v>1529</v>
       </c>
     </row>
-    <row r="109" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
         <v>9</v>
       </c>
@@ -8823,7 +8812,7 @@
       </c>
       <c r="N111"/>
     </row>
-    <row r="112" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
         <v>9</v>
       </c>
@@ -8856,7 +8845,7 @@
       </c>
       <c r="N112"/>
     </row>
-    <row r="113" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
         <v>9</v>
       </c>
@@ -8889,7 +8878,7 @@
       </c>
       <c r="N113"/>
     </row>
-    <row r="114" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
         <v>9</v>
       </c>
@@ -8922,7 +8911,7 @@
       </c>
       <c r="N114"/>
     </row>
-    <row r="115" spans="1:14" ht="64" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
         <v>9</v>
       </c>
@@ -8955,7 +8944,7 @@
       </c>
       <c r="N115"/>
     </row>
-    <row r="116" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
         <v>9</v>
       </c>
@@ -8988,7 +8977,7 @@
       </c>
       <c r="N116"/>
     </row>
-    <row r="117" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
         <v>9</v>
       </c>
@@ -9056,7 +9045,7 @@
         <v>1531</v>
       </c>
     </row>
-    <row r="119" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
         <v>9</v>
       </c>
@@ -9091,7 +9080,7 @@
         <v>1532</v>
       </c>
     </row>
-    <row r="120" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
         <v>9</v>
       </c>
@@ -9124,7 +9113,7 @@
       </c>
       <c r="N120"/>
     </row>
-    <row r="121" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
         <v>9</v>
       </c>
@@ -9157,7 +9146,7 @@
       </c>
       <c r="N121"/>
     </row>
-    <row r="122" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
         <v>9</v>
       </c>
@@ -9189,7 +9178,7 @@
         <v>1533</v>
       </c>
     </row>
-    <row r="123" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
         <v>9</v>
       </c>
@@ -9219,7 +9208,7 @@
       </c>
       <c r="N123"/>
     </row>
-    <row r="124" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
         <v>9</v>
       </c>
@@ -9249,7 +9238,7 @@
       </c>
       <c r="N124"/>
     </row>
-    <row r="125" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
         <v>9</v>
       </c>
@@ -9276,7 +9265,7 @@
       </c>
       <c r="N125"/>
     </row>
-    <row r="126" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
         <v>9</v>
       </c>
@@ -9306,7 +9295,7 @@
       </c>
       <c r="N126"/>
     </row>
-    <row r="127" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
         <v>9</v>
       </c>
@@ -9336,7 +9325,7 @@
       </c>
       <c r="N127"/>
     </row>
-    <row r="128" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
         <v>9</v>
       </c>
@@ -9366,7 +9355,7 @@
       </c>
       <c r="N128"/>
     </row>
-    <row r="129" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A129" s="3" t="s">
         <v>9</v>
       </c>
@@ -9395,7 +9384,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="130" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="s">
         <v>9</v>
       </c>
@@ -9424,7 +9413,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="131" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
         <v>9</v>
       </c>
@@ -9453,7 +9442,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="132" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="s">
         <v>9</v>
       </c>
@@ -9482,7 +9471,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="133" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
         <v>9</v>
       </c>
@@ -9511,7 +9500,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="134" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
         <v>9</v>
       </c>
@@ -9540,7 +9529,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="135" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
         <v>9</v>
       </c>
@@ -9569,7 +9558,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="136" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A136" s="3" t="s">
         <v>9</v>
       </c>
@@ -9598,7 +9587,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="137" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A137" s="3" t="s">
         <v>9</v>
       </c>
@@ -9627,7 +9616,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="138" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A138" s="3" t="s">
         <v>9</v>
       </c>
@@ -9656,7 +9645,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="139" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A139" s="3" t="s">
         <v>9</v>
       </c>
@@ -9685,7 +9674,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="140" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A140" s="3" t="s">
         <v>9</v>
       </c>
@@ -9714,7 +9703,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="141" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A141" s="3" t="s">
         <v>9</v>
       </c>
@@ -9743,7 +9732,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="142" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A142" s="3" t="s">
         <v>9</v>
       </c>
@@ -9772,7 +9761,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="143" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A143" s="3" t="s">
         <v>9</v>
       </c>
@@ -9801,7 +9790,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="144" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A144" s="3" t="s">
         <v>9</v>
       </c>
@@ -9830,7 +9819,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="145" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A145" s="3" t="s">
         <v>9</v>
       </c>
@@ -9859,7 +9848,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="146" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A146" s="3" t="s">
         <v>9</v>
       </c>
@@ -9888,7 +9877,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="147" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A147" s="3" t="s">
         <v>9</v>
       </c>
@@ -9917,7 +9906,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="148" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A148" s="3" t="s">
         <v>9</v>
       </c>
@@ -9946,7 +9935,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="149" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A149" s="3" t="s">
         <v>9</v>
       </c>
@@ -9975,7 +9964,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="150" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A150" s="3" t="s">
         <v>9</v>
       </c>
@@ -10004,7 +9993,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="151" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A151" s="3" t="s">
         <v>9</v>
       </c>
@@ -10033,7 +10022,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="152" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A152" s="3" t="s">
         <v>9</v>
       </c>
@@ -10062,7 +10051,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="153" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A153" s="3" t="s">
         <v>9</v>
       </c>
@@ -10091,7 +10080,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="154" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A154" s="3" t="s">
         <v>9</v>
       </c>
@@ -10120,7 +10109,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="155" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A155" s="3" t="s">
         <v>9</v>
       </c>
@@ -10149,7 +10138,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="156" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A156" s="3" t="s">
         <v>9</v>
       </c>
@@ -10178,7 +10167,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="157" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A157" s="3" t="s">
         <v>9</v>
       </c>
@@ -10207,7 +10196,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="158" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A158" s="3" t="s">
         <v>9</v>
       </c>
@@ -10236,7 +10225,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="159" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A159" s="3" t="s">
         <v>9</v>
       </c>
@@ -10265,7 +10254,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="160" spans="1:9" customFormat="1" ht="80" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:9" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A160" s="3" t="s">
         <v>9</v>
       </c>
@@ -10294,7 +10283,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="161" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A161" s="3" t="s">
         <v>9</v>
       </c>
@@ -10323,7 +10312,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="162" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A162" s="3" t="s">
         <v>9</v>
       </c>
@@ -10352,7 +10341,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="163" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A163" s="3" t="s">
         <v>9</v>
       </c>
@@ -10381,7 +10370,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="164" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A164" s="3" t="s">
         <v>9</v>
       </c>
@@ -10410,7 +10399,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="165" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A165" s="3" t="s">
         <v>9</v>
       </c>
@@ -10439,7 +10428,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="166" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A166" s="3" t="s">
         <v>9</v>
       </c>
@@ -10468,7 +10457,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="167" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A167" s="3" t="s">
         <v>9</v>
       </c>
@@ -10497,7 +10486,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="168" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A168" s="3" t="s">
         <v>9</v>
       </c>
@@ -10524,7 +10513,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="169" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A169" s="3" t="s">
         <v>9</v>
       </c>
@@ -10553,7 +10542,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="170" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A170" s="3" t="s">
         <v>9</v>
       </c>
@@ -10582,7 +10571,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="171" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A171" s="3" t="s">
         <v>9</v>
       </c>
@@ -10611,7 +10600,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="172" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A172" s="3" t="s">
         <v>9</v>
       </c>
@@ -10640,7 +10629,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="173" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A173" s="3" t="s">
         <v>9</v>
       </c>
@@ -10669,7 +10658,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="174" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A174" s="3" t="s">
         <v>9</v>
       </c>
@@ -10698,7 +10687,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="175" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A175" s="3" t="s">
         <v>9</v>
       </c>
@@ -10727,7 +10716,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="176" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A176" s="3" t="s">
         <v>9</v>
       </c>
@@ -10756,7 +10745,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="177" spans="1:9" customFormat="1" ht="64" hidden="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:9" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A177" s="3" t="s">
         <v>9</v>
       </c>
@@ -10785,7 +10774,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="178" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A178" s="3" t="s">
         <v>9</v>
       </c>
@@ -10814,7 +10803,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="179" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A179" s="3" t="s">
         <v>9</v>
       </c>
@@ -10843,7 +10832,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="180" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A180" s="3" t="s">
         <v>9</v>
       </c>
@@ -10872,7 +10861,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="181" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A181" s="3" t="s">
         <v>9</v>
       </c>
@@ -10901,7 +10890,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="182" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A182" s="3" t="s">
         <v>9</v>
       </c>
@@ -10930,7 +10919,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="183" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A183" s="3" t="s">
         <v>9</v>
       </c>
@@ -10959,7 +10948,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="184" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A184" s="3" t="s">
         <v>9</v>
       </c>
@@ -10988,7 +10977,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="185" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A185" s="3" t="s">
         <v>9</v>
       </c>
@@ -11017,7 +11006,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="186" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A186" s="3" t="s">
         <v>9</v>
       </c>
@@ -11046,7 +11035,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="187" spans="1:9" customFormat="1" ht="64" hidden="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:9" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A187" s="3" t="s">
         <v>9</v>
       </c>
@@ -11075,7 +11064,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="188" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A188" s="3" t="s">
         <v>9</v>
       </c>
@@ -11104,7 +11093,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="189" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A189" s="3" t="s">
         <v>9</v>
       </c>
@@ -11133,7 +11122,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="190" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A190" s="3" t="s">
         <v>9</v>
       </c>
@@ -11162,7 +11151,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="191" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A191" s="3" t="s">
         <v>9</v>
       </c>
@@ -11191,7 +11180,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="192" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A192" s="3" t="s">
         <v>9</v>
       </c>
@@ -11220,7 +11209,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="193" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A193" s="3" t="s">
         <v>9</v>
       </c>
@@ -11249,7 +11238,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="194" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A194" s="3" t="s">
         <v>9</v>
       </c>
@@ -11278,7 +11267,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="195" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A195" s="3" t="s">
         <v>9</v>
       </c>
@@ -11307,7 +11296,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="196" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A196" s="3" t="s">
         <v>9</v>
       </c>
@@ -11336,7 +11325,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="197" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A197" s="3" t="s">
         <v>9</v>
       </c>
@@ -11365,7 +11354,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="198" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A198" s="3" t="s">
         <v>9</v>
       </c>
@@ -11394,7 +11383,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="199" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A199" s="3" t="s">
         <v>9</v>
       </c>
@@ -11423,7 +11412,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="200" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A200" s="3" t="s">
         <v>9</v>
       </c>
@@ -11452,7 +11441,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="201" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A201" s="3" t="s">
         <v>9</v>
       </c>
@@ -11479,7 +11468,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="202" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A202" s="3" t="s">
         <v>9</v>
       </c>
@@ -11508,7 +11497,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="203" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A203" s="3" t="s">
         <v>9</v>
       </c>
@@ -11537,7 +11526,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="204" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A204" s="3" t="s">
         <v>9</v>
       </c>
@@ -11566,7 +11555,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="205" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A205" s="3" t="s">
         <v>9</v>
       </c>
@@ -11595,7 +11584,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="206" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A206" s="3" t="s">
         <v>9</v>
       </c>
@@ -11624,7 +11613,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="207" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A207" s="3" t="s">
         <v>9</v>
       </c>
@@ -11653,7 +11642,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="208" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A208" s="3" t="s">
         <v>9</v>
       </c>
@@ -11682,7 +11671,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="209" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A209" s="3" t="s">
         <v>9</v>
       </c>
@@ -11711,7 +11700,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="210" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A210" s="3" t="s">
         <v>9</v>
       </c>
@@ -11738,7 +11727,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="211" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A211" s="3" t="s">
         <v>9</v>
       </c>
@@ -11767,7 +11756,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="212" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A212" s="3" t="s">
         <v>9</v>
       </c>
@@ -11794,7 +11783,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="213" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A213" s="3" t="s">
         <v>9</v>
       </c>
@@ -11823,7 +11812,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="214" spans="1:9" customFormat="1" ht="64" hidden="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:9" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A214" s="3" t="s">
         <v>9</v>
       </c>
@@ -11852,7 +11841,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="215" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A215" s="3" t="s">
         <v>9</v>
       </c>
@@ -11881,7 +11870,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="216" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A216" s="3" t="s">
         <v>9</v>
       </c>
@@ -11910,7 +11899,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="217" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A217" s="3" t="s">
         <v>9</v>
       </c>
@@ -11937,7 +11926,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="218" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A218" s="3" t="s">
         <v>9</v>
       </c>
@@ -11966,7 +11955,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="219" spans="1:9" customFormat="1" ht="64" hidden="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:9" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A219" s="3" t="s">
         <v>9</v>
       </c>
@@ -11995,7 +11984,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="220" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A220" s="3" t="s">
         <v>9</v>
       </c>
@@ -12024,7 +12013,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="221" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A221" s="3" t="s">
         <v>9</v>
       </c>
@@ -12053,7 +12042,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="222" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A222" s="3" t="s">
         <v>9</v>
       </c>
@@ -12082,7 +12071,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="223" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A223" s="3" t="s">
         <v>9</v>
       </c>
@@ -12111,7 +12100,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="224" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A224" s="3" t="s">
         <v>9</v>
       </c>
@@ -12140,7 +12129,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="225" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A225" s="3" t="s">
         <v>9</v>
       </c>
@@ -12167,7 +12156,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="226" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A226" s="3" t="s">
         <v>9</v>
       </c>
@@ -12196,7 +12185,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="227" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A227" s="3" t="s">
         <v>9</v>
       </c>
@@ -12225,7 +12214,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="228" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A228" s="3" t="s">
         <v>9</v>
       </c>
@@ -12254,7 +12243,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="229" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A229" s="3" t="s">
         <v>9</v>
       </c>
@@ -12283,7 +12272,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="230" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A230" s="3" t="s">
         <v>9</v>
       </c>
@@ -12312,7 +12301,7 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="231" spans="1:9" customFormat="1" ht="64" hidden="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:9" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A231" s="3" t="s">
         <v>9</v>
       </c>
@@ -12341,7 +12330,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="232" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A232" s="3" t="s">
         <v>9</v>
       </c>
@@ -12370,7 +12359,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="233" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A233" s="3" t="s">
         <v>9</v>
       </c>
@@ -12399,7 +12388,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="234" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A234" s="3" t="s">
         <v>9</v>
       </c>
@@ -12428,7 +12417,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="235" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A235" s="3" t="s">
         <v>9</v>
       </c>
@@ -12457,7 +12446,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="236" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A236" s="3" t="s">
         <v>9</v>
       </c>
@@ -12486,7 +12475,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="237" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A237" s="3" t="s">
         <v>9</v>
       </c>
@@ -12515,7 +12504,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="238" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A238" s="3" t="s">
         <v>9</v>
       </c>
@@ -12544,7 +12533,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="239" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A239" s="3" t="s">
         <v>9</v>
       </c>
@@ -12573,7 +12562,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="240" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A240" s="3" t="s">
         <v>9</v>
       </c>
@@ -12602,7 +12591,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="241" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A241" s="3" t="s">
         <v>9</v>
       </c>
@@ -12631,7 +12620,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="242" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A242" s="3" t="s">
         <v>9</v>
       </c>
@@ -12660,7 +12649,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="243" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A243" s="3" t="s">
         <v>9</v>
       </c>
@@ -12689,7 +12678,7 @@
         <v>1069</v>
       </c>
     </row>
-    <row r="244" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A244" s="3" t="s">
         <v>9</v>
       </c>
@@ -12718,7 +12707,7 @@
         <v>1074</v>
       </c>
     </row>
-    <row r="245" spans="1:9" customFormat="1" ht="64" hidden="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:9" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A245" s="3" t="s">
         <v>9</v>
       </c>
@@ -12747,7 +12736,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="246" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A246" s="3" t="s">
         <v>9</v>
       </c>
@@ -12776,7 +12765,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="247" spans="1:9" customFormat="1" ht="64" hidden="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:9" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A247" s="3" t="s">
         <v>9</v>
       </c>
@@ -12805,7 +12794,7 @@
         <v>1089</v>
       </c>
     </row>
-    <row r="248" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A248" s="3" t="s">
         <v>9</v>
       </c>
@@ -12834,7 +12823,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="249" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A249" s="3" t="s">
         <v>9</v>
       </c>
@@ -12861,7 +12850,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="250" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A250" s="3" t="s">
         <v>9</v>
       </c>
@@ -12890,7 +12879,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="251" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A251" s="3" t="s">
         <v>9</v>
       </c>
@@ -12919,7 +12908,7 @@
         <v>1106</v>
       </c>
     </row>
-    <row r="252" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A252" s="3" t="s">
         <v>9</v>
       </c>
@@ -12948,7 +12937,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="253" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A253" s="3" t="s">
         <v>9</v>
       </c>
@@ -12977,7 +12966,7 @@
         <v>1114</v>
       </c>
     </row>
-    <row r="254" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A254" s="3" t="s">
         <v>9</v>
       </c>
@@ -13006,7 +12995,7 @@
         <v>1119</v>
       </c>
     </row>
-    <row r="255" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A255" s="3" t="s">
         <v>9</v>
       </c>
@@ -13035,7 +13024,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="256" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A256" s="3" t="s">
         <v>9</v>
       </c>
@@ -13064,7 +13053,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="257" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A257" s="3" t="s">
         <v>9</v>
       </c>
@@ -13093,7 +13082,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="258" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A258" s="3" t="s">
         <v>9</v>
       </c>
@@ -13122,7 +13111,7 @@
         <v>1137</v>
       </c>
     </row>
-    <row r="259" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A259" s="3" t="s">
         <v>9</v>
       </c>
@@ -13151,7 +13140,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="260" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A260" s="3" t="s">
         <v>9</v>
       </c>
@@ -13180,7 +13169,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="261" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A261" s="3" t="s">
         <v>9</v>
       </c>
@@ -13209,7 +13198,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="262" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A262" s="3" t="s">
         <v>9</v>
       </c>
@@ -13238,7 +13227,7 @@
         <v>1154</v>
       </c>
     </row>
-    <row r="263" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A263" s="3" t="s">
         <v>9</v>
       </c>
@@ -13267,7 +13256,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="264" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A264" s="3" t="s">
         <v>9</v>
       </c>
@@ -13296,7 +13285,7 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="265" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A265" s="3" t="s">
         <v>9</v>
       </c>
@@ -13325,7 +13314,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="266" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A266" s="3" t="s">
         <v>9</v>
       </c>
@@ -13354,7 +13343,7 @@
         <v>1172</v>
       </c>
     </row>
-    <row r="267" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A267" s="3" t="s">
         <v>9</v>
       </c>
@@ -13383,7 +13372,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="268" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A268" s="3" t="s">
         <v>9</v>
       </c>
@@ -13412,7 +13401,7 @@
         <v>1182</v>
       </c>
     </row>
-    <row r="269" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A269" s="3" t="s">
         <v>9</v>
       </c>
@@ -13439,7 +13428,7 @@
         <v>1186</v>
       </c>
     </row>
-    <row r="270" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A270" s="3" t="s">
         <v>9</v>
       </c>
@@ -13468,7 +13457,7 @@
         <v>1190</v>
       </c>
     </row>
-    <row r="271" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A271" s="3" t="s">
         <v>9</v>
       </c>
@@ -13497,7 +13486,7 @@
         <v>1195</v>
       </c>
     </row>
-    <row r="272" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A272" s="3" t="s">
         <v>9</v>
       </c>
@@ -13526,7 +13515,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="273" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A273" s="3" t="s">
         <v>9</v>
       </c>
@@ -13555,7 +13544,7 @@
         <v>1205</v>
       </c>
     </row>
-    <row r="274" spans="1:9" customFormat="1" ht="64" hidden="1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:9" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A274" s="3" t="s">
         <v>9</v>
       </c>
@@ -13584,7 +13573,7 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="275" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A275" s="3" t="s">
         <v>9</v>
       </c>
@@ -13613,7 +13602,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="276" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A276" s="3" t="s">
         <v>9</v>
       </c>
@@ -13642,7 +13631,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="277" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A277" s="3" t="s">
         <v>9</v>
       </c>
@@ -13671,7 +13660,7 @@
         <v>1221</v>
       </c>
     </row>
-    <row r="278" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A278" s="3" t="s">
         <v>9</v>
       </c>
@@ -13700,7 +13689,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="279" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A279" s="3" t="s">
         <v>9</v>
       </c>
@@ -13729,7 +13718,7 @@
         <v>1229</v>
       </c>
     </row>
-    <row r="280" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A280" s="3" t="s">
         <v>9</v>
       </c>
@@ -13758,7 +13747,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="281" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A281" s="3" t="s">
         <v>9</v>
       </c>
@@ -13787,7 +13776,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="282" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A282" s="3" t="s">
         <v>9</v>
       </c>
@@ -13816,7 +13805,7 @@
         <v>1241</v>
       </c>
     </row>
-    <row r="283" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A283" s="3" t="s">
         <v>9</v>
       </c>
@@ -13845,7 +13834,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="284" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A284" s="3" t="s">
         <v>9</v>
       </c>
@@ -13874,7 +13863,7 @@
         <v>1251</v>
       </c>
     </row>
-    <row r="285" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A285" s="3" t="s">
         <v>9</v>
       </c>
@@ -13903,7 +13892,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="286" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A286" s="3" t="s">
         <v>9</v>
       </c>
@@ -13930,7 +13919,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="287" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A287" s="3" t="s">
         <v>9</v>
       </c>
@@ -13957,7 +13946,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="288" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A288" s="3" t="s">
         <v>9</v>
       </c>
@@ -13986,7 +13975,7 @@
         <v>1268</v>
       </c>
     </row>
-    <row r="289" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A289" s="3" t="s">
         <v>9</v>
       </c>
@@ -14015,7 +14004,7 @@
         <v>1273</v>
       </c>
     </row>
-    <row r="290" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A290" s="3" t="s">
         <v>9</v>
       </c>
@@ -14044,7 +14033,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="291" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A291" s="3" t="s">
         <v>9</v>
       </c>
@@ -14073,7 +14062,7 @@
         <v>1283</v>
       </c>
     </row>
-    <row r="292" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A292" s="3" t="s">
         <v>9</v>
       </c>
@@ -14102,7 +14091,7 @@
         <v>1287</v>
       </c>
     </row>
-    <row r="293" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A293" s="3" t="s">
         <v>9</v>
       </c>
@@ -14131,7 +14120,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="294" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A294" s="3" t="s">
         <v>9</v>
       </c>
@@ -14160,7 +14149,7 @@
         <v>1294</v>
       </c>
     </row>
-    <row r="295" spans="1:9" customFormat="1" ht="64" hidden="1" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:9" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A295" s="3" t="s">
         <v>9</v>
       </c>
@@ -14189,7 +14178,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="296" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A296" s="3" t="s">
         <v>9</v>
       </c>
@@ -14218,7 +14207,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="297" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A297" s="3" t="s">
         <v>9</v>
       </c>
@@ -14247,7 +14236,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="298" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A298" s="3" t="s">
         <v>9</v>
       </c>
@@ -14274,7 +14263,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="299" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A299" s="3" t="s">
         <v>9</v>
       </c>
@@ -14303,7 +14292,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="300" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A300" s="3" t="s">
         <v>9</v>
       </c>
@@ -14330,7 +14319,7 @@
         <v>1316</v>
       </c>
     </row>
-    <row r="301" spans="1:9" customFormat="1" ht="64" hidden="1" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:9" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A301" s="3" t="s">
         <v>9</v>
       </c>
@@ -14359,7 +14348,7 @@
         <v>1321</v>
       </c>
     </row>
-    <row r="302" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A302" s="3" t="s">
         <v>9</v>
       </c>
@@ -14388,7 +14377,7 @@
         <v>1326</v>
       </c>
     </row>
-    <row r="303" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A303" s="3" t="s">
         <v>9</v>
       </c>
@@ -14417,7 +14406,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="304" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A304" s="3" t="s">
         <v>9</v>
       </c>
@@ -14446,7 +14435,7 @@
         <v>1335</v>
       </c>
     </row>
-    <row r="305" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A305" s="3" t="s">
         <v>9</v>
       </c>
@@ -14475,7 +14464,7 @@
         <v>1339</v>
       </c>
     </row>
-    <row r="306" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A306" s="3" t="s">
         <v>9</v>
       </c>
@@ -14504,7 +14493,7 @@
         <v>1344</v>
       </c>
     </row>
-    <row r="307" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A307" s="3" t="s">
         <v>9</v>
       </c>
@@ -14533,7 +14522,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="308" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A308" s="3" t="s">
         <v>9</v>
       </c>
@@ -14562,7 +14551,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="309" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A309" s="3" t="s">
         <v>9</v>
       </c>
@@ -14591,7 +14580,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="310" spans="1:9" customFormat="1" ht="64" hidden="1" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:9" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A310" s="3" t="s">
         <v>9</v>
       </c>
@@ -14620,7 +14609,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="311" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A311" s="3" t="s">
         <v>9</v>
       </c>
@@ -14649,7 +14638,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="312" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A312" s="3" t="s">
         <v>9</v>
       </c>
@@ -14678,7 +14667,7 @@
         <v>1367</v>
       </c>
     </row>
-    <row r="313" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A313" s="3" t="s">
         <v>9</v>
       </c>
@@ -14707,7 +14696,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="314" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A314" s="3" t="s">
         <v>9</v>
       </c>
@@ -14736,7 +14725,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="315" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A315" s="3" t="s">
         <v>9</v>
       </c>
@@ -14765,7 +14754,7 @@
         <v>1379</v>
       </c>
     </row>
-    <row r="316" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A316" s="3" t="s">
         <v>9</v>
       </c>
@@ -14794,7 +14783,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="317" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A317" s="3" t="s">
         <v>9</v>
       </c>
@@ -14823,7 +14812,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="318" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A318" s="3" t="s">
         <v>9</v>
       </c>
@@ -14852,7 +14841,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="319" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A319" s="3" t="s">
         <v>9</v>
       </c>
@@ -14881,7 +14870,7 @@
         <v>1397</v>
       </c>
     </row>
-    <row r="320" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A320" s="3" t="s">
         <v>9</v>
       </c>
@@ -14910,7 +14899,7 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="321" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A321" s="3" t="s">
         <v>9</v>
       </c>
@@ -14939,7 +14928,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="322" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A322" s="3" t="s">
         <v>9</v>
       </c>
@@ -14968,7 +14957,7 @@
         <v>1411</v>
       </c>
     </row>
-    <row r="323" spans="1:9" customFormat="1" ht="64" hidden="1" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:9" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A323" s="3" t="s">
         <v>9</v>
       </c>
@@ -14997,7 +14986,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="324" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A324" s="3" t="s">
         <v>9</v>
       </c>
@@ -15026,7 +15015,7 @@
         <v>1420</v>
       </c>
     </row>
-    <row r="325" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A325" s="3" t="s">
         <v>9</v>
       </c>
@@ -15055,7 +15044,7 @@
         <v>1425</v>
       </c>
     </row>
-    <row r="326" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A326" s="3" t="s">
         <v>9</v>
       </c>
@@ -15082,7 +15071,7 @@
         <v>1186</v>
       </c>
     </row>
-    <row r="327" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A327" s="3" t="s">
         <v>9</v>
       </c>
@@ -15109,7 +15098,7 @@
         <v>1186</v>
       </c>
     </row>
-    <row r="328" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A328" s="3" t="s">
         <v>9</v>
       </c>
@@ -15136,7 +15125,7 @@
         <v>1186</v>
       </c>
     </row>
-    <row r="329" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A329" s="3" t="s">
         <v>9</v>
       </c>
@@ -15165,7 +15154,7 @@
         <v>1437</v>
       </c>
     </row>
-    <row r="330" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A330" s="3" t="s">
         <v>9</v>
       </c>
@@ -15194,7 +15183,7 @@
         <v>1442</v>
       </c>
     </row>
-    <row r="331" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A331" s="3" t="s">
         <v>9</v>
       </c>
@@ -15223,7 +15212,7 @@
         <v>1447</v>
       </c>
     </row>
-    <row r="332" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A332" s="3" t="s">
         <v>9</v>
       </c>
@@ -15252,7 +15241,7 @@
         <v>1452</v>
       </c>
     </row>
-    <row r="333" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A333" s="3" t="s">
         <v>9</v>
       </c>
@@ -15281,7 +15270,7 @@
         <v>1456</v>
       </c>
     </row>
-    <row r="334" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A334" s="3" t="s">
         <v>9</v>
       </c>
@@ -15310,7 +15299,7 @@
         <v>1461</v>
       </c>
     </row>
-    <row r="335" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A335" s="3" t="s">
         <v>9</v>
       </c>
@@ -15339,7 +15328,7 @@
         <v>1466</v>
       </c>
     </row>
-    <row r="336" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A336" s="3" t="s">
         <v>9</v>
       </c>
@@ -15368,7 +15357,7 @@
         <v>1470</v>
       </c>
     </row>
-    <row r="337" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A337" s="3" t="s">
         <v>9</v>
       </c>
@@ -15397,7 +15386,7 @@
         <v>1475</v>
       </c>
     </row>
-    <row r="338" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A338" s="3" t="s">
         <v>9</v>
       </c>
@@ -15426,7 +15415,7 @@
         <v>1480</v>
       </c>
     </row>
-    <row r="339" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A339" s="3" t="s">
         <v>9</v>
       </c>
@@ -15455,7 +15444,7 @@
         <v>1485</v>
       </c>
     </row>
-    <row r="340" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A340" s="3" t="s">
         <v>9</v>
       </c>
@@ -15484,7 +15473,7 @@
         <v>1490</v>
       </c>
     </row>
-    <row r="341" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A341" s="3" t="s">
         <v>9</v>
       </c>
@@ -15513,7 +15502,7 @@
         <v>1495</v>
       </c>
     </row>
-    <row r="342" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A342" s="3" t="s">
         <v>9</v>
       </c>
@@ -15542,7 +15531,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="343" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A343" s="3" t="s">
         <v>9</v>
       </c>
@@ -15571,7 +15560,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="344" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A344" s="3" t="s">
         <v>9</v>
       </c>

</xml_diff>